<commit_message>
[FIXUP] Force close on some events [FIXUP] Remove field jabatan when login type is 0 [REMOVE] Add/Remove row button [ADD] Status when data already exists [ADD] Import excel thread [ADD] Excel file format validation [ADD] Row highlight on current data uploading
</commit_message>
<xml_diff>
--- a/template/IPNU-Anggota-Nama_PAC-Nama_Ranting_Komsat.xlsx
+++ b/template/IPNU-Anggota-Nama_PAC-Nama_Ranting_Komsat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patur/Workdir/research/conthongev1.0.0/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2607A16B-4D65-4D4C-B89B-116D80D5B911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD12478D-00EC-044F-B78A-8FA5C4CE8F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="33820" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>PP</t>
   </si>
   <si>
-    <t>Cbp</t>
-  </si>
-  <si>
     <t>Pendidikan</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>samidiuyeee@gmail.com</t>
+  </si>
+  <si>
+    <t>Cbp/Kpp</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1239,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1254,7 +1254,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -1266,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -1278,7 +1278,7 @@
         <v>13</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>14</v>
@@ -1290,10 +1290,10 @@
         <v>16</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>17</v>
@@ -1302,22 +1302,22 @@
         <v>18</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>19</v>
@@ -1334,103 +1334,103 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2">
         <v>35682</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
         <v>63</v>
-      </c>
-      <c r="L2" t="s">
-        <v>64</v>
       </c>
       <c r="M2" s="2">
         <v>41099</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
         <v>65</v>
-      </c>
-      <c r="P2" t="s">
-        <v>66</v>
       </c>
       <c r="Q2" s="2">
         <v>41916</v>
       </c>
       <c r="R2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" t="s">
         <v>77</v>
-      </c>
-      <c r="T2" t="s">
-        <v>78</v>
       </c>
       <c r="U2" s="2">
         <v>41916</v>
       </c>
       <c r="V2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" t="s">
         <v>67</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>68</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>70</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>71</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF2" t="s">
         <v>72</v>
       </c>
-      <c r="AC2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>73</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>74</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
@@ -1781,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -1795,7 +1795,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1806,10 +1806,10 @@
         <v>25</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1820,10 +1820,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1834,10 +1834,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1845,10 +1845,10 @@
         <v>30</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1856,10 +1856,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1867,10 +1867,10 @@
         <v>29</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1878,81 +1878,81 @@
         <v>31</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIXUP] Force close on some events [FIXUP] Remove field jabatan when login type is 0 [REMOVE] Add/Remove row button [ADD] Status when data already exists [ADD] Import excel thread [ADD] Excel file format validation
</commit_message>
<xml_diff>
--- a/template/IPNU-Anggota-Nama_PAC-Nama_Ranting_Komsat.xlsx
+++ b/template/IPNU-Anggota-Nama_PAC-Nama_Ranting_Komsat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patur/Workdir/research/conthongev1.0.0/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2607A16B-4D65-4D4C-B89B-116D80D5B911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD12478D-00EC-044F-B78A-8FA5C4CE8F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="500" windowWidth="33820" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -119,9 +119,6 @@
     <t>PP</t>
   </si>
   <si>
-    <t>Cbp</t>
-  </si>
-  <si>
     <t>Pendidikan</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>samidiuyeee@gmail.com</t>
+  </si>
+  <si>
+    <t>Cbp/Kpp</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1239,7 +1239,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1254,7 +1254,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>
@@ -1266,7 +1266,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
@@ -1278,7 +1278,7 @@
         <v>13</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>14</v>
@@ -1290,10 +1290,10 @@
         <v>16</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>32</v>
+        <v>97</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>17</v>
@@ -1302,22 +1302,22 @@
         <v>18</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="AE1" s="4" t="s">
         <v>19</v>
@@ -1334,103 +1334,103 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2">
         <v>35682</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
         <v>63</v>
-      </c>
-      <c r="L2" t="s">
-        <v>64</v>
       </c>
       <c r="M2" s="2">
         <v>41099</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" t="s">
         <v>65</v>
-      </c>
-      <c r="P2" t="s">
-        <v>66</v>
       </c>
       <c r="Q2" s="2">
         <v>41916</v>
       </c>
       <c r="R2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" t="s">
         <v>77</v>
-      </c>
-      <c r="T2" t="s">
-        <v>78</v>
       </c>
       <c r="U2" s="2">
         <v>41916</v>
       </c>
       <c r="V2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" t="s">
         <v>67</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>68</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" t="s">
         <v>69</v>
       </c>
-      <c r="Y2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>70</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>71</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF2" t="s">
         <v>72</v>
       </c>
-      <c r="AC2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>73</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>74</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
@@ -1781,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -1795,7 +1795,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1806,10 +1806,10 @@
         <v>25</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1820,10 +1820,10 @@
         <v>26</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1834,10 +1834,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1845,10 +1845,10 @@
         <v>30</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1856,10 +1856,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1867,10 +1867,10 @@
         <v>29</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1878,81 +1878,81 @@
         <v>31</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>